<commit_message>
Attached all line chart in the email body
</commit_message>
<xml_diff>
--- a/Data/sku_wise_target_sales.xlsx
+++ b/Data/sku_wise_target_sales.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,16 +476,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>393142096.62</v>
+        <v>477386831.61</v>
       </c>
       <c r="D2" t="n">
-        <v>17462235.84</v>
+        <v>29716069.6</v>
       </c>
       <c r="E2" t="n">
-        <v>11926.062</v>
+        <v>13645.134</v>
       </c>
       <c r="F2" t="n">
-        <v>35076</v>
+        <v>59690</v>
       </c>
     </row>
     <row r="3">
@@ -498,16 +498,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>804875454</v>
+        <v>1363305138</v>
       </c>
       <c r="D3" t="n">
-        <v>12535966.48</v>
+        <v>20027118.3</v>
       </c>
       <c r="E3" t="n">
-        <v>499317.264</v>
+        <v>848663.634</v>
       </c>
       <c r="F3" t="n">
-        <v>15741.856</v>
+        <v>25148.76</v>
       </c>
     </row>
     <row r="4">
@@ -520,16 +520,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>440499400.5</v>
+        <v>798975810</v>
       </c>
       <c r="D4" t="n">
-        <v>8361672.84</v>
+        <v>15161443.3</v>
       </c>
       <c r="E4" t="n">
-        <v>446260.986</v>
+        <v>953873.036</v>
       </c>
       <c r="F4" t="n">
-        <v>10500.048</v>
+        <v>19038.76</v>
       </c>
     </row>
     <row r="5">
@@ -542,302 +542,302 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>54606261.6</v>
+        <v>140045089.2</v>
       </c>
       <c r="D5" t="n">
-        <v>623293.4399999999</v>
+        <v>2089866.24</v>
       </c>
       <c r="E5" t="n">
-        <v>48617.28</v>
+        <v>153289.872</v>
       </c>
       <c r="F5" t="n">
-        <v>1413.72</v>
+        <v>4740.12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Kurkure Large (45 gm) - CC</t>
+          <t>Kurkure Large (45 gm) - MM</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>34072464.2</v>
+        <v>55874725.28</v>
       </c>
       <c r="D6" t="n">
-        <v>586629.12</v>
+        <v>1704890.88</v>
       </c>
       <c r="E6" t="n">
-        <v>18474.24</v>
+        <v>62366.172</v>
       </c>
       <c r="F6" t="n">
-        <v>1330.56</v>
+        <v>3866.94</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kurkure Large (45 gm) - MM</t>
+          <t>Lays (25 gm) - STT</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>19690619.83</v>
+        <v>79585686</v>
       </c>
       <c r="D7" t="n">
-        <v>366643.2</v>
+        <v>1615014</v>
       </c>
       <c r="E7" t="n">
-        <v>16205.16</v>
+        <v>101235.432</v>
       </c>
       <c r="F7" t="n">
-        <v>831.6</v>
+        <v>1950.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>215</v>
+        <v>166</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Lays Pastazz - 37 gm (Poly)</t>
+          <t>Lays(25 gm) ASCO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>21173958.72</v>
+        <v>126078225</v>
       </c>
       <c r="D8" t="n">
-        <v>343533.96</v>
+        <v>1615014</v>
       </c>
       <c r="E8" t="n">
-        <v>26082.144</v>
+        <v>137464.6</v>
       </c>
       <c r="F8" t="n">
-        <v>747.252</v>
+        <v>1950.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Lays Pastazz - 20 gm</t>
+          <t>Kurkure Large (45 gm) - CC</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>24164365.68</v>
+        <v>80504617.2</v>
       </c>
       <c r="D9" t="n">
-        <v>257499</v>
+        <v>1264919.04</v>
       </c>
       <c r="E9" t="n">
-        <v>76540.46400000001</v>
+        <v>35556.528</v>
       </c>
       <c r="F9" t="n">
-        <v>545.292</v>
+        <v>2869.02</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>166</v>
+        <v>213</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Lays(25 gm) ASCO</t>
+          <t>Lays 3D-37 gm (Poly)</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>50664406.5</v>
+        <v>18093323.04</v>
       </c>
       <c r="D10" t="n">
-        <v>235483.2</v>
+        <v>1204988.4</v>
       </c>
       <c r="E10" t="n">
-        <v>27952.776</v>
+        <v>78005.928</v>
       </c>
       <c r="F10" t="n">
-        <v>284.4</v>
+        <v>2621.08</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>142</v>
+        <v>216</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Kurkure (20 gm) - Chilli Chatka</t>
+          <t>Lays Pastazz - 20 gm</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>47394018.14</v>
+        <v>113853749.4</v>
       </c>
       <c r="D11" t="n">
-        <v>225813.6</v>
+        <v>942310</v>
       </c>
       <c r="E11" t="n">
-        <v>73151.46000000001</v>
+        <v>341405.42</v>
       </c>
       <c r="F11" t="n">
-        <v>568.8</v>
+        <v>1995.48</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Kurkure (90 gm) - Masala Munch</t>
+          <t>Kurkure (45 gm) - STT</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1443282.12</v>
+        <v>27437588.45</v>
       </c>
       <c r="D12" t="n">
-        <v>225699.84</v>
+        <v>895180.8</v>
       </c>
       <c r="E12" t="n">
-        <v>623.448</v>
+        <v>50581.056</v>
       </c>
       <c r="F12" t="n">
-        <v>511.92</v>
+        <v>2030.4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Kurkure (90 gm) - ASCO</t>
+          <t>Kurkure (20 gm)- ASCO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3764676.15</v>
+        <v>353070781.84</v>
       </c>
       <c r="D13" t="n">
-        <v>206891.52</v>
+        <v>828459.6</v>
       </c>
       <c r="E13" t="n">
-        <v>993.795</v>
+        <v>672112.1040000001</v>
       </c>
       <c r="F13" t="n">
-        <v>469.26</v>
+        <v>2086.8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>199</v>
+        <v>142</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Quaker Oats (500 gm Jar)</t>
+          <t>Kurkure (20 gm) - Chilli Chatka</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>23936164.56</v>
+        <v>144274267.2</v>
       </c>
       <c r="D14" t="n">
-        <v>203333.9</v>
+        <v>716505.6</v>
       </c>
       <c r="E14" t="n">
-        <v>143.88</v>
+        <v>221693.952</v>
       </c>
       <c r="F14" t="n">
-        <v>385</v>
+        <v>1804.8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Lays (25 gm) - STT</t>
+          <t>Kurkure (90 gm) - STT</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>25232871</v>
+        <v>1671383.7</v>
       </c>
       <c r="D15" t="n">
-        <v>170071.2</v>
+        <v>671385.6</v>
       </c>
       <c r="E15" t="n">
-        <v>15081.716</v>
+        <v>2887.92</v>
       </c>
       <c r="F15" t="n">
-        <v>205.4</v>
+        <v>1522.8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>154</v>
+        <v>215</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Kurkure (90 gm) - Chilli Chatka</t>
+          <t>Lays Pastazz - 37 gm (Poly)</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1043083.44</v>
+        <v>61251584.4</v>
       </c>
       <c r="D16" t="n">
-        <v>169274.88</v>
+        <v>641617.2</v>
       </c>
       <c r="E16" t="n">
-        <v>337.932</v>
+        <v>62493.84</v>
       </c>
       <c r="F16" t="n">
-        <v>383.94</v>
+        <v>1395.64</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Kurkure (20 gm)- ASCO</t>
+          <t>Kurkure (20 gm) - Masala Munch</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>66704574.16</v>
+        <v>234505493.6</v>
       </c>
       <c r="D17" t="n">
-        <v>150542.4</v>
+        <v>559770</v>
       </c>
       <c r="E17" t="n">
-        <v>120116.28</v>
+        <v>222252</v>
       </c>
       <c r="F17" t="n">
-        <v>379.2</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>143</v>
+        <v>199</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Kurkure (20 gm) - Masala Munch</t>
+          <t>Quaker Oats (500 gm Jar)</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>61715445.61</v>
+        <v>59237349.15</v>
       </c>
       <c r="D18" t="n">
-        <v>135488.16</v>
+        <v>549001.53</v>
       </c>
       <c r="E18" t="n">
-        <v>61550.172</v>
+        <v>384.561</v>
       </c>
       <c r="F18" t="n">
-        <v>341.28</v>
+        <v>1039.5</v>
       </c>
     </row>
     <row r="19">
@@ -850,103 +850,185 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>19406009.49</v>
+        <v>148290535.05</v>
       </c>
       <c r="D19" t="n">
-        <v>60216.96</v>
+        <v>425425.2</v>
       </c>
       <c r="E19" t="n">
-        <v>37274.448</v>
+        <v>270590.172</v>
       </c>
       <c r="F19" t="n">
-        <v>151.68</v>
+        <v>1071.6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>213</v>
+        <v>155</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Lays 3D-37 gm (Poly)</t>
+          <t>Kurkure (90 gm) - Masala Munch</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5769994.48</v>
+        <v>2020411.62</v>
       </c>
       <c r="D20" t="n">
-        <v>57255.66</v>
+        <v>335692.8</v>
       </c>
       <c r="E20" t="n">
-        <v>3553.748</v>
+        <v>872.748</v>
       </c>
       <c r="F20" t="n">
-        <v>124.542</v>
+        <v>761.4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>198</v>
+        <v>157</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kurkure Large (45 gm) - TJM</t>
+          <t>Kurkure (90 gm) - ASCO</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>76133.64999999999</v>
+        <v>6362383.95</v>
       </c>
       <c r="D21" t="n">
-        <v>36664.32</v>
+        <v>307718.4</v>
       </c>
       <c r="E21" t="n">
-        <v>43.86</v>
+        <v>1679.535</v>
       </c>
       <c r="F21" t="n">
-        <v>83.16</v>
+        <v>697.95</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Kurkure (20 gm) - Tock Misti Jhal</t>
+          <t>Kurkure (90 gm) - Chilli Chatka</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>10645.74</v>
+        <v>1620212.94</v>
       </c>
       <c r="D22" t="n">
-        <v>15054.24</v>
+        <v>251769.6</v>
       </c>
       <c r="E22" t="n">
-        <v>15.336</v>
+        <v>524.907</v>
       </c>
       <c r="F22" t="n">
-        <v>37.92</v>
+        <v>571.05</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
+        <v>198</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Kurkure Large (45 gm) - TJM</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1935023.68</v>
+      </c>
+      <c r="D23" t="n">
+        <v>219985.92</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1114.752</v>
+      </c>
+      <c r="F23" t="n">
+        <v>498.96</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>144</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Kurkure (20 gm) - Tock Misti Jhal</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>5189623.32</v>
+      </c>
+      <c r="D24" t="n">
+        <v>134344.8</v>
+      </c>
+      <c r="E24" t="n">
+        <v>7476.048</v>
+      </c>
+      <c r="F24" t="n">
+        <v>338.4</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>217</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Lays 3D - 20 gm</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>5719548.91</v>
+      </c>
+      <c r="D25" t="n">
+        <v>13005</v>
+      </c>
+      <c r="E25" t="n">
+        <v>6404.87</v>
+      </c>
+      <c r="F25" t="n">
+        <v>27.54</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
         <v>156</v>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>Kurkure (90 gm) - Tock Misti Jhal</t>
         </is>
       </c>
-      <c r="C23" t="n">
-        <v>50004</v>
-      </c>
-      <c r="D23" t="n">
+      <c r="C27" t="n">
+        <v>593547.48</v>
+      </c>
+      <c r="D27" t="n">
         <v>0</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E27" t="n">
         <v>0</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F27" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update and Finalize design layout
</commit_message>
<xml_diff>
--- a/Data/sku_wise_target_sales.xlsx
+++ b/Data/sku_wise_target_sales.xlsx
@@ -437,22 +437,22 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>SKUID</t>
+          <t>Item</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>SKU Name</t>
+          <t>skuname</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Months Sales Target(Tk)</t>
+          <t>Months Target(Tk)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>MTD Sales Target(Tk)</t>
+          <t>MTD Target(Tk)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -462,27 +462,27 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Value Achiv %</t>
+          <t>Months Target(Kg)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Months Volume Target(Kg)</t>
+          <t>MTD Target(Kg)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>MTD Volume Target(Kg)</t>
+          <t>MTD Sales(Kg)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Sales Volume(Kg)</t>
+          <t>Achiv%(Tk)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Volume Achiv %</t>
+          <t>Achiv%(Kg)</t>
         </is>
       </c>
     </row>
@@ -496,28 +496,28 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>177938263</v>
+        <v>20866.65</v>
       </c>
       <c r="D2" t="n">
-        <v>103318991</v>
+        <v>13462</v>
       </c>
       <c r="E2" t="n">
-        <v>895632</v>
+        <v>4287.6</v>
       </c>
       <c r="F2" t="n">
-        <v>0.86</v>
+        <v>50.1</v>
       </c>
       <c r="G2" t="n">
-        <v>277117</v>
+        <v>32</v>
       </c>
       <c r="H2" t="n">
-        <v>160907</v>
+        <v>10.8</v>
       </c>
       <c r="I2" t="n">
-        <v>2256</v>
+        <v>31.84965086911306</v>
       </c>
       <c r="J2" t="n">
-        <v>1.4</v>
+        <v>33.75</v>
       </c>
     </row>
     <row r="3">
@@ -530,810 +530,810 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>296217466</v>
+        <v>20866.65</v>
       </c>
       <c r="D3" t="n">
-        <v>171997238</v>
+        <v>13462</v>
       </c>
       <c r="E3" t="n">
-        <v>716506</v>
+        <v>1381.56</v>
       </c>
       <c r="F3" t="n">
-        <v>0.41</v>
+        <v>50.1</v>
       </c>
       <c r="G3" t="n">
-        <v>284483</v>
+        <v>32</v>
       </c>
       <c r="H3" t="n">
-        <v>165183</v>
+        <v>3.48</v>
       </c>
       <c r="I3" t="n">
-        <v>1805</v>
+        <v>10.26266528004754</v>
       </c>
       <c r="J3" t="n">
-        <v>1.09</v>
+        <v>10.875</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Kurkure (20 gm) - STT</t>
+          <t>Kurkure (20 gm) - Tock Misti Jhal</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>177948642</v>
+        <v>12519.99</v>
       </c>
       <c r="D4" t="n">
-        <v>103325018</v>
+        <v>8077</v>
       </c>
       <c r="E4" t="n">
-        <v>492598</v>
+        <v>666.96</v>
       </c>
       <c r="F4" t="n">
-        <v>0.47</v>
+        <v>30.06</v>
       </c>
       <c r="G4" t="n">
-        <v>313315</v>
+        <v>19</v>
       </c>
       <c r="H4" t="n">
-        <v>181925</v>
+        <v>1.68</v>
       </c>
       <c r="I4" t="n">
-        <v>1241</v>
+        <v>8.257521356939458</v>
       </c>
       <c r="J4" t="n">
-        <v>0.68</v>
+        <v>8.842105263157894</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Kurkure (20 gm) - Tock Misti Jhal</t>
+          <t>Kurkure (20 gm)- ASCO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6054561</v>
+        <v>62608.28</v>
       </c>
       <c r="D5" t="n">
-        <v>3515551</v>
+        <v>40392</v>
       </c>
       <c r="E5" t="n">
-        <v>156736</v>
+        <v>5335.68</v>
       </c>
       <c r="F5" t="n">
-        <v>4.45</v>
+        <v>150.32</v>
       </c>
       <c r="G5" t="n">
-        <v>8722</v>
+        <v>97</v>
       </c>
       <c r="H5" t="n">
-        <v>5064</v>
+        <v>13.44</v>
       </c>
       <c r="I5" t="n">
-        <v>395</v>
+        <v>13.20974450386215</v>
       </c>
       <c r="J5" t="n">
-        <v>7.79</v>
+        <v>13.85567010309278</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Kurkure (20 gm)- ASCO</t>
+          <t>Kurkure (90 gm) - Chilli Chatka</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>479167490</v>
+        <v>4208.67</v>
       </c>
       <c r="D6" t="n">
-        <v>278226284</v>
+        <v>2715</v>
       </c>
       <c r="E6" t="n">
-        <v>1074758</v>
+        <v>1944.32</v>
       </c>
       <c r="F6" t="n">
-        <v>0.38</v>
+        <v>9.09</v>
       </c>
       <c r="G6" t="n">
-        <v>871929</v>
+        <v>6</v>
       </c>
       <c r="H6" t="n">
-        <v>506281</v>
+        <v>4.41</v>
       </c>
       <c r="I6" t="n">
-        <v>2707</v>
+        <v>71.61399631675874</v>
       </c>
       <c r="J6" t="n">
-        <v>0.53</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kurkure (45 gm) - STT</t>
+          <t>Kurkure (90 gm) - Masala Munch</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>27437588</v>
+        <v>4208.67</v>
       </c>
       <c r="D7" t="n">
-        <v>15931503</v>
+        <v>2715</v>
       </c>
       <c r="E7" t="n">
-        <v>895181</v>
+        <v>2301.44</v>
       </c>
       <c r="F7" t="n">
-        <v>5.61</v>
+        <v>9.09</v>
       </c>
       <c r="G7" t="n">
-        <v>50581</v>
+        <v>6</v>
       </c>
       <c r="H7" t="n">
-        <v>29370</v>
+        <v>5.22</v>
       </c>
       <c r="I7" t="n">
-        <v>2030</v>
+        <v>84.76758747697974</v>
       </c>
       <c r="J7" t="n">
-        <v>6.91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Kurkure (90 gm) - ASCO</t>
+          <t>Kurkure (90 gm) - Tock Misti Jhal</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>14845563</v>
+        <v>2541.87</v>
       </c>
       <c r="D8" t="n">
-        <v>8620004</v>
+        <v>1640</v>
       </c>
       <c r="E8" t="n">
-        <v>867206</v>
+        <v>79.36</v>
       </c>
       <c r="F8" t="n">
-        <v>10.06</v>
+        <v>5.49</v>
       </c>
       <c r="G8" t="n">
-        <v>4733</v>
+        <v>4</v>
       </c>
       <c r="H8" t="n">
-        <v>2748</v>
+        <v>0.18</v>
       </c>
       <c r="I8" t="n">
-        <v>1967</v>
+        <v>4.839024390243902</v>
       </c>
       <c r="J8" t="n">
-        <v>71.56</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Kurkure (90 gm) - Chilli Chatka</t>
+          <t>Kurkure (90 gm) - ASCO</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4050532</v>
+        <v>12667.68</v>
       </c>
       <c r="D9" t="n">
-        <v>2351922</v>
+        <v>8173</v>
       </c>
       <c r="E9" t="n">
-        <v>456915</v>
+        <v>3690.24</v>
       </c>
       <c r="F9" t="n">
-        <v>19.42</v>
+        <v>27.36</v>
       </c>
       <c r="G9" t="n">
-        <v>953</v>
+        <v>18</v>
       </c>
       <c r="H9" t="n">
-        <v>553</v>
+        <v>8.369999999999999</v>
       </c>
       <c r="I9" t="n">
-        <v>1036</v>
+        <v>45.15159672091031</v>
       </c>
       <c r="J9" t="n">
-        <v>187.36</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Kurkure (90 gm) - Masala Munch</t>
+          <t>Kurkure (20 gm) - STT</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>5051029</v>
+        <v>50088.29</v>
       </c>
       <c r="D10" t="n">
-        <v>2932856</v>
+        <v>32315</v>
       </c>
       <c r="E10" t="n">
-        <v>540838</v>
+        <v>2096.16</v>
       </c>
       <c r="F10" t="n">
-        <v>18.44</v>
+        <v>120.26</v>
       </c>
       <c r="G10" t="n">
-        <v>1406</v>
+        <v>78</v>
       </c>
       <c r="H10" t="n">
-        <v>816</v>
+        <v>5.28</v>
       </c>
       <c r="I10" t="n">
-        <v>1227</v>
+        <v>6.486647067925112</v>
       </c>
       <c r="J10" t="n">
-        <v>150.24</v>
+        <v>6.769230769230769</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Kurkure (90 gm) - STT</t>
+          <t>Kurkure (45 gm) - STT</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>5014151</v>
+        <v>23892.01</v>
       </c>
       <c r="D11" t="n">
-        <v>2911443</v>
+        <v>15414</v>
       </c>
       <c r="E11" t="n">
-        <v>764634</v>
+        <v>3809.28</v>
       </c>
       <c r="F11" t="n">
-        <v>26.26</v>
+        <v>51.615</v>
       </c>
       <c r="G11" t="n">
-        <v>3289</v>
+        <v>33</v>
       </c>
       <c r="H11" t="n">
-        <v>1910</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="I11" t="n">
-        <v>1734</v>
+        <v>24.71311794472558</v>
       </c>
       <c r="J11" t="n">
-        <v>90.81</v>
+        <v>26.18181818181818</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Kurkure (90 gm) - Tock Misti Jhal</t>
+          <t>Kurkure (90 gm) - STT</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1187095</v>
+        <v>10167.48</v>
       </c>
       <c r="D12" t="n">
-        <v>689281</v>
+        <v>6560</v>
       </c>
       <c r="E12" t="n">
-        <v>205146</v>
+        <v>3253.76</v>
       </c>
       <c r="F12" t="n">
-        <v>29.76</v>
+        <v>21.96</v>
       </c>
       <c r="G12" t="n">
-        <v>104</v>
+        <v>14</v>
       </c>
       <c r="H12" t="n">
-        <v>61</v>
+        <v>7.38</v>
       </c>
       <c r="I12" t="n">
-        <v>465</v>
+        <v>49.60000000000001</v>
       </c>
       <c r="J12" t="n">
-        <v>767.17</v>
+        <v>52.71428571428572</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>195</v>
+        <v>166</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Kurkure Large (45 gm) - ASCO</t>
+          <t>Lays(25 gm) ASCO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>210067634</v>
+        <v>8221.5</v>
       </c>
       <c r="D13" t="n">
-        <v>121974755</v>
+        <v>5304</v>
       </c>
       <c r="E13" t="n">
-        <v>3024806</v>
+        <v>6582.6</v>
       </c>
       <c r="F13" t="n">
-        <v>2.47</v>
+        <v>9.449999999999999</v>
       </c>
       <c r="G13" t="n">
-        <v>221867</v>
+        <v>6</v>
       </c>
       <c r="H13" t="n">
-        <v>128826</v>
+        <v>7.95</v>
       </c>
       <c r="I13" t="n">
-        <v>6861</v>
+        <v>124.106334841629</v>
       </c>
       <c r="J13" t="n">
-        <v>5.32</v>
+        <v>132.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Kurkure Large (45 gm) - CC</t>
+          <t>Lays (25 gm) - STT</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>112706464</v>
+        <v>4741.5</v>
       </c>
       <c r="D14" t="n">
-        <v>65442463</v>
+        <v>3059</v>
       </c>
       <c r="E14" t="n">
-        <v>1778220</v>
+        <v>7493.4</v>
       </c>
       <c r="F14" t="n">
-        <v>2.71</v>
+        <v>5.45</v>
       </c>
       <c r="G14" t="n">
-        <v>49985</v>
+        <v>4</v>
       </c>
       <c r="H14" t="n">
-        <v>29024</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="I14" t="n">
-        <v>4033</v>
+        <v>244.9624060150376</v>
       </c>
       <c r="J14" t="n">
-        <v>13.89</v>
+        <v>226.25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Kurkure Large (45 gm) - MM</t>
+          <t>Lays(52 gm) ASCO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>80319918</v>
+        <v>167692.5</v>
       </c>
       <c r="D15" t="n">
-        <v>46637372</v>
+        <v>108189</v>
       </c>
       <c r="E15" t="n">
-        <v>2218191</v>
+        <v>64019.86</v>
       </c>
       <c r="F15" t="n">
-        <v>4.75</v>
+        <v>200.46</v>
       </c>
       <c r="G15" t="n">
-        <v>81143</v>
+        <v>129</v>
       </c>
       <c r="H15" t="n">
-        <v>47115</v>
+        <v>80.392</v>
       </c>
       <c r="I15" t="n">
-        <v>5031</v>
+        <v>59.17409348455018</v>
       </c>
       <c r="J15" t="n">
-        <v>10.67</v>
+        <v>62.31937984496124</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Kurkure Large (45 gm) - TJM</t>
+          <t>Lays (52 gm) - STT</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3386291</v>
+        <v>96744</v>
       </c>
       <c r="D16" t="n">
-        <v>1966234</v>
+        <v>62415</v>
       </c>
       <c r="E16" t="n">
-        <v>348311</v>
+        <v>117521.58</v>
       </c>
       <c r="F16" t="n">
-        <v>17.71</v>
+        <v>115.648</v>
       </c>
       <c r="G16" t="n">
-        <v>1765</v>
+        <v>75</v>
       </c>
       <c r="H16" t="n">
-        <v>1025</v>
+        <v>147.576</v>
       </c>
       <c r="I16" t="n">
-        <v>790</v>
+        <v>188.2906032203797</v>
       </c>
       <c r="J16" t="n">
-        <v>77.08</v>
+        <v>196.768</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Lays (25 gm) - STT</t>
+          <t>Quaker Oats (1000gm)</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>92849967</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>53912884</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>1760949</v>
+        <v>132425.44</v>
       </c>
       <c r="F17" t="n">
-        <v>3.26</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>110383</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>64093</v>
+        <v>266</v>
       </c>
       <c r="I17" t="n">
-        <v>2127</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>3.31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>172</v>
+        <v>195</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Lays (52 gm) - STT</t>
+          <t>Kurkure Large (45 gm) - ASCO</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1650316746</v>
+        <v>29870.22</v>
       </c>
       <c r="D18" t="n">
-        <v>958248433</v>
+        <v>19271</v>
       </c>
       <c r="E18" t="n">
-        <v>26994765</v>
+        <v>13332.48</v>
       </c>
       <c r="F18" t="n">
-        <v>2.81</v>
+        <v>64.53</v>
       </c>
       <c r="G18" t="n">
-        <v>1143923</v>
+        <v>42</v>
       </c>
       <c r="H18" t="n">
-        <v>664213</v>
+        <v>30.24</v>
       </c>
       <c r="I18" t="n">
-        <v>33898</v>
+        <v>69.18416273156555</v>
       </c>
       <c r="J18" t="n">
-        <v>5.1</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Lays 3D - 20 gm</t>
+          <t>Kurkure Large (45 gm) - CC</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>28597745</v>
+        <v>9956.74</v>
       </c>
       <c r="D19" t="n">
-        <v>16605142</v>
+        <v>6424</v>
       </c>
       <c r="E19" t="n">
-        <v>78030</v>
+        <v>4920.32</v>
       </c>
       <c r="F19" t="n">
-        <v>0.46</v>
+        <v>21.51</v>
       </c>
       <c r="G19" t="n">
-        <v>38429</v>
+        <v>14</v>
       </c>
       <c r="H19" t="n">
-        <v>22314</v>
+        <v>11.16</v>
       </c>
       <c r="I19" t="n">
-        <v>165</v>
+        <v>76.59277708592776</v>
       </c>
       <c r="J19" t="n">
-        <v>0.74</v>
+        <v>79.71428571428572</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Lays 3D-37 gm (Poly)</t>
+          <t>Kurkure Large (45 gm) - MM</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>22616654</v>
+        <v>9956.74</v>
       </c>
       <c r="D20" t="n">
-        <v>13132251</v>
+        <v>6424</v>
       </c>
       <c r="E20" t="n">
-        <v>1291059</v>
+        <v>9602.559999999999</v>
       </c>
       <c r="F20" t="n">
-        <v>9.83</v>
+        <v>21.51</v>
       </c>
       <c r="G20" t="n">
-        <v>83578</v>
+        <v>14</v>
       </c>
       <c r="H20" t="n">
-        <v>48529</v>
+        <v>21.78</v>
       </c>
       <c r="I20" t="n">
-        <v>2808</v>
+        <v>149.4794520547945</v>
       </c>
       <c r="J20" t="n">
-        <v>5.78</v>
+        <v>155.5714285714286</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Lays Pastazz - 20 gm</t>
+          <t>Kurkure Large (45 gm) - TJM</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>145479791</v>
+        <v>5978.21</v>
       </c>
       <c r="D21" t="n">
-        <v>84472137</v>
+        <v>3857</v>
       </c>
       <c r="E21" t="n">
-        <v>1040060</v>
+        <v>1507.84</v>
       </c>
       <c r="F21" t="n">
-        <v>1.23</v>
+        <v>12.915</v>
       </c>
       <c r="G21" t="n">
-        <v>376821</v>
+        <v>8</v>
       </c>
       <c r="H21" t="n">
-        <v>218799</v>
+        <v>3.42</v>
       </c>
       <c r="I21" t="n">
-        <v>2202</v>
+        <v>39.0935960591133</v>
       </c>
       <c r="J21" t="n">
-        <v>1</v>
+        <v>42.75</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Lays Pastazz - 37 gm (Poly)</t>
+          <t>Quaker Oats (500 gm Jar)</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>88474511</v>
+        <v>56840.35</v>
       </c>
       <c r="D22" t="n">
-        <v>51372297</v>
+        <v>36671</v>
       </c>
       <c r="E22" t="n">
-        <v>942864</v>
+        <v>8186.17</v>
       </c>
       <c r="F22" t="n">
-        <v>1.83</v>
+        <v>102.5</v>
       </c>
       <c r="G22" t="n">
-        <v>91835</v>
+        <v>66</v>
       </c>
       <c r="H22" t="n">
-        <v>53324</v>
+        <v>15.5</v>
       </c>
       <c r="I22" t="n">
-        <v>2051</v>
+        <v>22.32327997600284</v>
       </c>
       <c r="J22" t="n">
-        <v>3.84</v>
+        <v>23.48484848484848</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>166</v>
+        <v>213</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Lays(25 gm) ASCO</t>
+          <t>Lays 3D-37 gm (Poly)</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>162100575</v>
+        <v>24003.84</v>
       </c>
       <c r="D23" t="n">
-        <v>94122915</v>
+        <v>15486</v>
       </c>
       <c r="E23" t="n">
-        <v>1906884</v>
+        <v>5613.3</v>
       </c>
       <c r="F23" t="n">
-        <v>2.02</v>
+        <v>49.728</v>
       </c>
       <c r="G23" t="n">
-        <v>162308</v>
+        <v>32</v>
       </c>
       <c r="H23" t="n">
-        <v>94243</v>
+        <v>12.21</v>
       </c>
       <c r="I23" t="n">
-        <v>2303</v>
+        <v>36.24757845796204</v>
       </c>
       <c r="J23" t="n">
-        <v>2.44</v>
+        <v>38.15625</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>170</v>
+        <v>215</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Lays(52 gm) ASCO</t>
+          <t>Lays Pastazz - 37 gm (Poly)</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>798975810</v>
+        <v>48025.54</v>
       </c>
       <c r="D24" t="n">
-        <v>463921438</v>
+        <v>30984</v>
       </c>
       <c r="E24" t="n">
-        <v>15161443</v>
+        <v>4043.2031</v>
       </c>
       <c r="F24" t="n">
-        <v>3.26</v>
+        <v>99.49299999999999</v>
       </c>
       <c r="G24" t="n">
-        <v>953873</v>
+        <v>64</v>
       </c>
       <c r="H24" t="n">
-        <v>553862</v>
+        <v>8.731999999999999</v>
       </c>
       <c r="I24" t="n">
-        <v>19039</v>
+        <v>13.04932578104829</v>
       </c>
       <c r="J24" t="n">
-        <v>3.43</v>
+        <v>13.64375</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Quaker Oats (1000gm)</t>
+          <t>Lays Pastazz - 20 gm</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>477386832</v>
+        <v>42104.95</v>
       </c>
       <c r="D25" t="n">
-        <v>277192354</v>
+        <v>27164</v>
       </c>
       <c r="E25" t="n">
-        <v>29716070</v>
+        <v>4250</v>
       </c>
       <c r="F25" t="n">
-        <v>10.72</v>
+        <v>84.87</v>
       </c>
       <c r="G25" t="n">
-        <v>13645</v>
+        <v>55</v>
       </c>
       <c r="H25" t="n">
-        <v>7923</v>
+        <v>9</v>
       </c>
       <c r="I25" t="n">
-        <v>59690</v>
+        <v>15.64570755411574</v>
       </c>
       <c r="J25" t="n">
-        <v>753.37</v>
+        <v>16.36363636363636</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Quaker Oats (500 gm Jar)</t>
+          <t>Lays 3D - 20 gm</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>82932289</v>
+        <v>21056.94</v>
       </c>
       <c r="D26" t="n">
-        <v>48154232</v>
+        <v>13585</v>
       </c>
       <c r="E26" t="n">
-        <v>1891005</v>
+        <v>510</v>
       </c>
       <c r="F26" t="n">
-        <v>3.92</v>
+        <v>42.444</v>
       </c>
       <c r="G26" t="n">
-        <v>1325</v>
+        <v>27</v>
       </c>
       <c r="H26" t="n">
-        <v>769</v>
+        <v>1.08</v>
       </c>
       <c r="I26" t="n">
-        <v>3581</v>
+        <v>3.754140596245859</v>
       </c>
       <c r="J26" t="n">
-        <v>465.53</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
@@ -1346,28 +1346,28 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>27861509</v>
+        <v>386297.47</v>
       </c>
       <c r="D27" t="n">
-        <v>16177650</v>
+        <v>249224</v>
       </c>
       <c r="E27" t="n">
-        <v>1828072</v>
+        <v>11948.184</v>
       </c>
       <c r="F27" t="n">
-        <v>11.29</v>
+        <v>739</v>
       </c>
       <c r="G27" t="n">
-        <v>1279</v>
+        <v>477</v>
       </c>
       <c r="H27" t="n">
-        <v>743</v>
+        <v>24</v>
       </c>
       <c r="I27" t="n">
-        <v>3672</v>
+        <v>4.794154656052386</v>
       </c>
       <c r="J27" t="n">
-        <v>494.37</v>
+        <v>5.031446540880504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add regular expression note
</commit_message>
<xml_diff>
--- a/Data/sku_wise_target_sales.xlsx
+++ b/Data/sku_wise_target_sales.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,878 +496,402 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20866.65</v>
+        <v>20849.99</v>
       </c>
       <c r="D2" t="n">
-        <v>16828</v>
+        <v>6053</v>
       </c>
       <c r="E2" t="n">
-        <v>1429.2</v>
+        <v>500.22</v>
       </c>
       <c r="F2" t="n">
-        <v>50.1</v>
+        <v>50.06</v>
       </c>
       <c r="G2" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="H2" t="n">
-        <v>3.6</v>
+        <v>1.26</v>
       </c>
       <c r="I2" t="n">
-        <v>8.492987877347279</v>
+        <v>8.264001321658682</v>
       </c>
       <c r="J2" t="n">
-        <v>9</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Kurkure (20 gm) - Masala Munch</t>
+          <t>Kurkure (20 gm) - STT</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>20866.65</v>
+        <v>50046.64</v>
       </c>
       <c r="D3" t="n">
-        <v>16828</v>
+        <v>14530</v>
       </c>
       <c r="E3" t="n">
-        <v>1381.56</v>
+        <v>571.6799999999999</v>
       </c>
       <c r="F3" t="n">
-        <v>50.1</v>
+        <v>120.16</v>
       </c>
       <c r="G3" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H3" t="n">
-        <v>3.48</v>
+        <v>1.44</v>
       </c>
       <c r="I3" t="n">
-        <v>8.209888281435703</v>
+        <v>3.934480385409497</v>
       </c>
       <c r="J3" t="n">
-        <v>8.699999999999999</v>
+        <v>4.114285714285714</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Kurkure (20 gm) - Tock Misti Jhal</t>
+          <t>Kurkure (45 gm) - STT</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>12519.99</v>
+        <v>23871.18</v>
       </c>
       <c r="D4" t="n">
-        <v>10097</v>
+        <v>6930</v>
       </c>
       <c r="E4" t="n">
-        <v>666.96</v>
+        <v>5952</v>
       </c>
       <c r="F4" t="n">
-        <v>30.06</v>
+        <v>51.57</v>
       </c>
       <c r="G4" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H4" t="n">
-        <v>1.68</v>
+        <v>13.5</v>
       </c>
       <c r="I4" t="n">
-        <v>6.60552639397841</v>
+        <v>85.88744588744589</v>
       </c>
       <c r="J4" t="n">
-        <v>6.999999999999999</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Kurkure (20 gm)- ASCO</t>
+          <t>Lays(52 gm) ASCO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>62608.28</v>
+        <v>139591.5</v>
       </c>
       <c r="D5" t="n">
-        <v>50491</v>
+        <v>40527</v>
       </c>
       <c r="E5" t="n">
-        <v>28202.88</v>
+        <v>18344.63</v>
       </c>
       <c r="F5" t="n">
-        <v>150.32</v>
+        <v>166.868</v>
       </c>
       <c r="G5" t="n">
-        <v>121</v>
+        <v>48</v>
       </c>
       <c r="H5" t="n">
-        <v>71.04000000000001</v>
+        <v>23.036</v>
       </c>
       <c r="I5" t="n">
-        <v>55.85724188469232</v>
+        <v>45.26520591210798</v>
       </c>
       <c r="J5" t="n">
-        <v>58.7107438016529</v>
+        <v>47.99166666666667</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Kurkure (90 gm) - Chilli Chatka</t>
+          <t>Lays (52 gm) - STT</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4208.67</v>
+        <v>73645.5</v>
       </c>
       <c r="D6" t="n">
-        <v>3394</v>
+        <v>21381</v>
       </c>
       <c r="E6" t="n">
-        <v>3452.16</v>
+        <v>2898.7</v>
       </c>
       <c r="F6" t="n">
-        <v>9.09</v>
+        <v>88.036</v>
       </c>
       <c r="G6" t="n">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="H6" t="n">
-        <v>7.83</v>
+        <v>3.64</v>
       </c>
       <c r="I6" t="n">
-        <v>101.713612256924</v>
+        <v>13.55736401477948</v>
       </c>
       <c r="J6" t="n">
-        <v>111.8571428571429</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>155</v>
+        <v>195</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kurkure (90 gm) - Masala Munch</t>
+          <t>Kurkure Large (45 gm) - ASCO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4208.67</v>
+        <v>29849.39</v>
       </c>
       <c r="D7" t="n">
-        <v>3394</v>
+        <v>8666</v>
       </c>
       <c r="E7" t="n">
-        <v>4364.8</v>
+        <v>50234.88</v>
       </c>
       <c r="F7" t="n">
-        <v>9.09</v>
+        <v>64.485</v>
       </c>
       <c r="G7" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="H7" t="n">
-        <v>9.9</v>
+        <v>113.94</v>
       </c>
       <c r="I7" t="n">
-        <v>128.6034177961108</v>
+        <v>579.6778213708747</v>
       </c>
       <c r="J7" t="n">
-        <v>141.4285714285714</v>
+        <v>599.6842105263158</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>156</v>
+        <v>196</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Kurkure (90 gm) - Tock Misti Jhal</t>
+          <t>Kurkure Large (45 gm) - CC</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2541.87</v>
+        <v>9956.74</v>
       </c>
       <c r="D8" t="n">
-        <v>2050</v>
+        <v>2891</v>
       </c>
       <c r="E8" t="n">
-        <v>-39.68</v>
+        <v>20514.56</v>
       </c>
       <c r="F8" t="n">
-        <v>5.49</v>
+        <v>21.51</v>
       </c>
       <c r="G8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.09</v>
+        <v>46.53</v>
       </c>
       <c r="I8" t="n">
-        <v>-1.935609756097561</v>
+        <v>709.6008301625735</v>
       </c>
       <c r="J8" t="n">
-        <v>-2.25</v>
+        <v>775.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>157</v>
+        <v>197</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Kurkure (90 gm) - ASCO</t>
+          <t>Kurkure Large (45 gm) - MM</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>12667.68</v>
+        <v>9956.74</v>
       </c>
       <c r="D9" t="n">
-        <v>10216</v>
+        <v>2891</v>
       </c>
       <c r="E9" t="n">
-        <v>9800.959999999999</v>
+        <v>11904</v>
       </c>
       <c r="F9" t="n">
-        <v>27.36</v>
+        <v>21.51</v>
       </c>
       <c r="G9" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="H9" t="n">
-        <v>22.23</v>
+        <v>27</v>
       </c>
       <c r="I9" t="n">
-        <v>95.93735317149569</v>
+        <v>411.760636457973</v>
       </c>
       <c r="J9" t="n">
-        <v>101.0454545454545</v>
+        <v>450</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>158</v>
+        <v>199</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Kurkure (20 gm) - STT</t>
+          <t>Quaker Oats (500 gm Jar)</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>50088.29</v>
+        <v>127544.2</v>
       </c>
       <c r="D10" t="n">
-        <v>40394</v>
+        <v>37029</v>
       </c>
       <c r="E10" t="n">
-        <v>2096.16</v>
+        <v>264.07</v>
       </c>
       <c r="F10" t="n">
-        <v>120.26</v>
+        <v>230</v>
       </c>
       <c r="G10" t="n">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="H10" t="n">
-        <v>5.28</v>
+        <v>0.5</v>
       </c>
       <c r="I10" t="n">
-        <v>5.189285537456057</v>
+        <v>0.7131437521942261</v>
       </c>
       <c r="J10" t="n">
-        <v>5.443298969072165</v>
+        <v>0.7462686567164178</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>159</v>
+        <v>216</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Kurkure (45 gm) - STT</t>
+          <t>Lays Pastazz - 20 gm</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>23892.01</v>
+        <v>42078.16</v>
       </c>
       <c r="D11" t="n">
-        <v>19268</v>
+        <v>12216</v>
       </c>
       <c r="E11" t="n">
-        <v>4047.36</v>
+        <v>680</v>
       </c>
       <c r="F11" t="n">
-        <v>51.615</v>
+        <v>94.23999999999999</v>
       </c>
       <c r="G11" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="H11" t="n">
-        <v>9.18</v>
+        <v>1.6</v>
       </c>
       <c r="I11" t="n">
-        <v>21.00560514843264</v>
+        <v>5.566470203012443</v>
       </c>
       <c r="J11" t="n">
-        <v>21.85714285714285</v>
+        <v>5.925925925925926</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>160</v>
+        <v>217</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Kurkure (90 gm) - STT</t>
+          <t>Lays 3D - 20 gm</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>10167.48</v>
+        <v>21039.08</v>
       </c>
       <c r="D12" t="n">
-        <v>8200</v>
+        <v>6108</v>
       </c>
       <c r="E12" t="n">
-        <v>3729.92</v>
+        <v>4658</v>
       </c>
       <c r="F12" t="n">
-        <v>21.96</v>
+        <v>47.12</v>
       </c>
       <c r="G12" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H12" t="n">
-        <v>8.460000000000001</v>
+        <v>10.96</v>
       </c>
       <c r="I12" t="n">
-        <v>45.48682926829268</v>
+        <v>76.26064178127046</v>
       </c>
       <c r="J12" t="n">
-        <v>47</v>
+        <v>78.28571428571429</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>166</v>
+        <v>220</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Lays(25 gm) ASCO</t>
+          <t>Lays(52 gm) Hot n Sweet Chilli</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>8221.5</v>
+        <v>54244.5</v>
       </c>
       <c r="D13" t="n">
-        <v>6630</v>
+        <v>15748</v>
       </c>
       <c r="E13" t="n">
-        <v>32478.3</v>
+        <v>1449.35</v>
       </c>
       <c r="F13" t="n">
-        <v>9.449999999999999</v>
+        <v>64.84399999999999</v>
       </c>
       <c r="G13" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="H13" t="n">
-        <v>39.225</v>
+        <v>1.82</v>
       </c>
       <c r="I13" t="n">
-        <v>489.868778280543</v>
+        <v>9.203390906781813</v>
       </c>
       <c r="J13" t="n">
-        <v>490.3125</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>168</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Lays (25 gm) - STT</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>4741.5</v>
-      </c>
-      <c r="D14" t="n">
-        <v>3824</v>
-      </c>
-      <c r="E14" t="n">
-        <v>10101.6</v>
-      </c>
-      <c r="F14" t="n">
-        <v>5.45</v>
-      </c>
-      <c r="G14" t="n">
-        <v>4</v>
-      </c>
-      <c r="H14" t="n">
-        <v>12.2</v>
-      </c>
-      <c r="I14" t="n">
-        <v>264.163179916318</v>
-      </c>
-      <c r="J14" t="n">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>170</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Lays(52 gm) ASCO</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>167692.5</v>
-      </c>
-      <c r="D15" t="n">
-        <v>135236</v>
-      </c>
-      <c r="E15" t="n">
-        <v>70645.46000000001</v>
-      </c>
-      <c r="F15" t="n">
-        <v>200.46</v>
-      </c>
-      <c r="G15" t="n">
-        <v>162</v>
-      </c>
-      <c r="H15" t="n">
-        <v>88.712</v>
-      </c>
-      <c r="I15" t="n">
-        <v>52.23864947203408</v>
-      </c>
-      <c r="J15" t="n">
-        <v>54.7604938271605</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>172</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Lays (52 gm) - STT</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>96744</v>
-      </c>
-      <c r="D16" t="n">
-        <v>78019</v>
-      </c>
-      <c r="E16" t="n">
-        <v>178063</v>
-      </c>
-      <c r="F16" t="n">
-        <v>115.648</v>
-      </c>
-      <c r="G16" t="n">
-        <v>93</v>
-      </c>
-      <c r="H16" t="n">
-        <v>223.6</v>
-      </c>
-      <c r="I16" t="n">
-        <v>228.2303028749407</v>
-      </c>
-      <c r="J16" t="n">
-        <v>240.4301075268817</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>187</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Quaker Oats (1000gm)</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" t="n">
-        <v>132425.44</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" t="n">
-        <v>266</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>195</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Kurkure Large (45 gm) - ASCO</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>29870.22</v>
-      </c>
-      <c r="D18" t="n">
-        <v>24089</v>
-      </c>
-      <c r="E18" t="n">
-        <v>14760.96</v>
-      </c>
-      <c r="F18" t="n">
-        <v>64.53</v>
-      </c>
-      <c r="G18" t="n">
-        <v>52</v>
-      </c>
-      <c r="H18" t="n">
-        <v>33.48</v>
-      </c>
-      <c r="I18" t="n">
-        <v>61.27676532857321</v>
-      </c>
-      <c r="J18" t="n">
-        <v>64.38461538461537</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>196</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Kurkure Large (45 gm) - CC</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>9956.74</v>
-      </c>
-      <c r="D19" t="n">
-        <v>8030</v>
-      </c>
-      <c r="E19" t="n">
-        <v>5773.44</v>
-      </c>
-      <c r="F19" t="n">
-        <v>21.51</v>
-      </c>
-      <c r="G19" t="n">
-        <v>17</v>
-      </c>
-      <c r="H19" t="n">
-        <v>13.095</v>
-      </c>
-      <c r="I19" t="n">
-        <v>71.8983810709838</v>
-      </c>
-      <c r="J19" t="n">
-        <v>77.02941176470588</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>197</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Kurkure Large (45 gm) - MM</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>9956.74</v>
-      </c>
-      <c r="D20" t="n">
-        <v>8030</v>
-      </c>
-      <c r="E20" t="n">
-        <v>10792.96</v>
-      </c>
-      <c r="F20" t="n">
-        <v>21.51</v>
-      </c>
-      <c r="G20" t="n">
-        <v>17</v>
-      </c>
-      <c r="H20" t="n">
-        <v>24.48</v>
-      </c>
-      <c r="I20" t="n">
-        <v>134.4079701120797</v>
-      </c>
-      <c r="J20" t="n">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>198</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Kurkure Large (45 gm) - TJM</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>5978.21</v>
-      </c>
-      <c r="D21" t="n">
-        <v>4821</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1507.84</v>
-      </c>
-      <c r="F21" t="n">
-        <v>12.915</v>
-      </c>
-      <c r="G21" t="n">
-        <v>10</v>
-      </c>
-      <c r="H21" t="n">
-        <v>3.42</v>
-      </c>
-      <c r="I21" t="n">
-        <v>31.27649865173201</v>
-      </c>
-      <c r="J21" t="n">
-        <v>34.2</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>199</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Quaker Oats (500 gm Jar)</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>56840.35</v>
-      </c>
-      <c r="D22" t="n">
-        <v>45839</v>
-      </c>
-      <c r="E22" t="n">
-        <v>119359.64</v>
-      </c>
-      <c r="F22" t="n">
-        <v>102.5</v>
-      </c>
-      <c r="G22" t="n">
-        <v>83</v>
-      </c>
-      <c r="H22" t="n">
-        <v>226</v>
-      </c>
-      <c r="I22" t="n">
-        <v>260.3888391980628</v>
-      </c>
-      <c r="J22" t="n">
-        <v>272.289156626506</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>213</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Lays 3D-37 gm (Poly)</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>24003.84</v>
-      </c>
-      <c r="D23" t="n">
-        <v>19358</v>
-      </c>
-      <c r="E23" t="n">
-        <v>5987.52</v>
-      </c>
-      <c r="F23" t="n">
-        <v>49.728</v>
-      </c>
-      <c r="G23" t="n">
-        <v>40</v>
-      </c>
-      <c r="H23" t="n">
-        <v>13.024</v>
-      </c>
-      <c r="I23" t="n">
-        <v>30.93046802355616</v>
-      </c>
-      <c r="J23" t="n">
-        <v>32.56</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>215</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Lays Pastazz - 37 gm (Poly)</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>48025.54</v>
-      </c>
-      <c r="D24" t="n">
-        <v>38730</v>
-      </c>
-      <c r="E24" t="n">
-        <v>5455.0331</v>
-      </c>
-      <c r="F24" t="n">
-        <v>99.49299999999999</v>
-      </c>
-      <c r="G24" t="n">
-        <v>80</v>
-      </c>
-      <c r="H24" t="n">
-        <v>11.803</v>
-      </c>
-      <c r="I24" t="n">
-        <v>14.08477433514072</v>
-      </c>
-      <c r="J24" t="n">
-        <v>14.75375</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>216</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Lays Pastazz - 20 gm</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>42104.95</v>
-      </c>
-      <c r="D25" t="n">
-        <v>33956</v>
-      </c>
-      <c r="E25" t="n">
-        <v>4250</v>
-      </c>
-      <c r="F25" t="n">
-        <v>84.87</v>
-      </c>
-      <c r="G25" t="n">
-        <v>68</v>
-      </c>
-      <c r="H25" t="n">
-        <v>9</v>
-      </c>
-      <c r="I25" t="n">
-        <v>12.51619743197078</v>
-      </c>
-      <c r="J25" t="n">
-        <v>13.23529411764706</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>217</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Lays 3D - 20 gm</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>21056.94</v>
-      </c>
-      <c r="D26" t="n">
-        <v>16981</v>
-      </c>
-      <c r="E26" t="n">
-        <v>510</v>
-      </c>
-      <c r="F26" t="n">
-        <v>42.444</v>
-      </c>
-      <c r="G26" t="n">
-        <v>34</v>
-      </c>
-      <c r="H26" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="I26" t="n">
-        <v>3.003356692774277</v>
-      </c>
-      <c r="J26" t="n">
-        <v>3.176470588235294</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>218</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Quaker Oats 1Kg New</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>386297.47</v>
-      </c>
-      <c r="D27" t="n">
-        <v>311530</v>
-      </c>
-      <c r="E27" t="n">
-        <v>29870.46</v>
-      </c>
-      <c r="F27" t="n">
-        <v>739</v>
-      </c>
-      <c r="G27" t="n">
-        <v>596</v>
-      </c>
-      <c r="H27" t="n">
-        <v>60</v>
-      </c>
-      <c r="I27" t="n">
-        <v>9.588309312104773</v>
-      </c>
-      <c r="J27" t="n">
-        <v>10.06711409395973</v>
+        <v>9.578947368421053</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update coding structure in dashboard.py
</commit_message>
<xml_diff>
--- a/Data/sku_wise_target_sales.xlsx
+++ b/Data/sku_wise_target_sales.xlsx
@@ -499,7 +499,7 @@
         <v>20849.99</v>
       </c>
       <c r="D2" t="n">
-        <v>6053</v>
+        <v>6726</v>
       </c>
       <c r="E2" t="n">
         <v>500.22</v>
@@ -508,16 +508,16 @@
         <v>50.06</v>
       </c>
       <c r="G2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" t="n">
         <v>1.26</v>
       </c>
       <c r="I2" t="n">
-        <v>8.264001321658682</v>
+        <v>7.437109723461195</v>
       </c>
       <c r="J2" t="n">
-        <v>8.4</v>
+        <v>7.875</v>
       </c>
     </row>
     <row r="3">
@@ -533,7 +533,7 @@
         <v>50046.64</v>
       </c>
       <c r="D3" t="n">
-        <v>14530</v>
+        <v>16144</v>
       </c>
       <c r="E3" t="n">
         <v>571.6799999999999</v>
@@ -542,16 +542,16 @@
         <v>120.16</v>
       </c>
       <c r="G3" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H3" t="n">
         <v>1.44</v>
       </c>
       <c r="I3" t="n">
-        <v>3.934480385409497</v>
+        <v>3.541129831516353</v>
       </c>
       <c r="J3" t="n">
-        <v>4.114285714285714</v>
+        <v>3.692307692307692</v>
       </c>
     </row>
     <row r="4">
@@ -567,7 +567,7 @@
         <v>23871.18</v>
       </c>
       <c r="D4" t="n">
-        <v>6930</v>
+        <v>7700</v>
       </c>
       <c r="E4" t="n">
         <v>5952</v>
@@ -576,16 +576,16 @@
         <v>51.57</v>
       </c>
       <c r="G4" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H4" t="n">
         <v>13.5</v>
       </c>
       <c r="I4" t="n">
-        <v>85.88744588744589</v>
+        <v>77.2987012987013</v>
       </c>
       <c r="J4" t="n">
-        <v>90</v>
+        <v>79.41176470588235</v>
       </c>
     </row>
     <row r="5">
@@ -601,7 +601,7 @@
         <v>139591.5</v>
       </c>
       <c r="D5" t="n">
-        <v>40527</v>
+        <v>45030</v>
       </c>
       <c r="E5" t="n">
         <v>18344.63</v>
@@ -610,16 +610,16 @@
         <v>166.868</v>
       </c>
       <c r="G5" t="n">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="H5" t="n">
         <v>23.036</v>
       </c>
       <c r="I5" t="n">
-        <v>45.26520591210798</v>
+        <v>40.73868532089718</v>
       </c>
       <c r="J5" t="n">
-        <v>47.99166666666667</v>
+        <v>42.65925925925927</v>
       </c>
     </row>
     <row r="6">
@@ -635,7 +635,7 @@
         <v>73645.5</v>
       </c>
       <c r="D6" t="n">
-        <v>21381</v>
+        <v>23757</v>
       </c>
       <c r="E6" t="n">
         <v>2898.7</v>
@@ -644,16 +644,16 @@
         <v>88.036</v>
       </c>
       <c r="G6" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H6" t="n">
         <v>3.64</v>
       </c>
       <c r="I6" t="n">
-        <v>13.55736401477948</v>
+        <v>12.20145641284674</v>
       </c>
       <c r="J6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -669,7 +669,7 @@
         <v>29849.39</v>
       </c>
       <c r="D7" t="n">
-        <v>8666</v>
+        <v>9629</v>
       </c>
       <c r="E7" t="n">
         <v>50234.88</v>
@@ -678,16 +678,16 @@
         <v>64.485</v>
       </c>
       <c r="G7" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H7" t="n">
         <v>113.94</v>
       </c>
       <c r="I7" t="n">
-        <v>579.6778213708747</v>
+        <v>521.7040191089417</v>
       </c>
       <c r="J7" t="n">
-        <v>599.6842105263158</v>
+        <v>542.5714285714286</v>
       </c>
     </row>
     <row r="8">
@@ -703,7 +703,7 @@
         <v>9956.74</v>
       </c>
       <c r="D8" t="n">
-        <v>2891</v>
+        <v>3212</v>
       </c>
       <c r="E8" t="n">
         <v>20514.56</v>
@@ -712,16 +712,16 @@
         <v>21.51</v>
       </c>
       <c r="G8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H8" t="n">
         <v>46.53</v>
       </c>
       <c r="I8" t="n">
-        <v>709.6008301625735</v>
+        <v>638.6849315068494</v>
       </c>
       <c r="J8" t="n">
-        <v>775.5</v>
+        <v>664.7142857142858</v>
       </c>
     </row>
     <row r="9">
@@ -737,7 +737,7 @@
         <v>9956.74</v>
       </c>
       <c r="D9" t="n">
-        <v>2891</v>
+        <v>3212</v>
       </c>
       <c r="E9" t="n">
         <v>11904</v>
@@ -746,16 +746,16 @@
         <v>21.51</v>
       </c>
       <c r="G9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H9" t="n">
         <v>27</v>
       </c>
       <c r="I9" t="n">
-        <v>411.760636457973</v>
+        <v>370.6102117061021</v>
       </c>
       <c r="J9" t="n">
-        <v>450</v>
+        <v>385.7142857142857</v>
       </c>
     </row>
     <row r="10">
@@ -771,7 +771,7 @@
         <v>127544.2</v>
       </c>
       <c r="D10" t="n">
-        <v>37029</v>
+        <v>41143</v>
       </c>
       <c r="E10" t="n">
         <v>264.07</v>
@@ -780,16 +780,16 @@
         <v>230</v>
       </c>
       <c r="G10" t="n">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="H10" t="n">
         <v>0.5</v>
       </c>
       <c r="I10" t="n">
-        <v>0.7131437521942261</v>
+        <v>0.6418345769632744</v>
       </c>
       <c r="J10" t="n">
-        <v>0.7462686567164178</v>
+        <v>0.6756756756756757</v>
       </c>
     </row>
     <row r="11">
@@ -805,7 +805,7 @@
         <v>42078.16</v>
       </c>
       <c r="D11" t="n">
-        <v>12216</v>
+        <v>13574</v>
       </c>
       <c r="E11" t="n">
         <v>680</v>
@@ -814,16 +814,16 @@
         <v>94.23999999999999</v>
       </c>
       <c r="G11" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H11" t="n">
         <v>1.6</v>
       </c>
       <c r="I11" t="n">
-        <v>5.566470203012443</v>
+        <v>5.009577132753794</v>
       </c>
       <c r="J11" t="n">
-        <v>5.925925925925926</v>
+        <v>5.333333333333334</v>
       </c>
     </row>
     <row r="12">
@@ -839,7 +839,7 @@
         <v>21039.08</v>
       </c>
       <c r="D12" t="n">
-        <v>6108</v>
+        <v>6787</v>
       </c>
       <c r="E12" t="n">
         <v>4658</v>
@@ -848,16 +848,16 @@
         <v>47.12</v>
       </c>
       <c r="G12" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12" t="n">
         <v>10.96</v>
       </c>
       <c r="I12" t="n">
-        <v>76.26064178127046</v>
+        <v>68.63120671872697</v>
       </c>
       <c r="J12" t="n">
-        <v>78.28571428571429</v>
+        <v>73.06666666666666</v>
       </c>
     </row>
     <row r="13">
@@ -873,7 +873,7 @@
         <v>54244.5</v>
       </c>
       <c r="D13" t="n">
-        <v>15748</v>
+        <v>17498</v>
       </c>
       <c r="E13" t="n">
         <v>1449.35</v>
@@ -882,16 +882,16 @@
         <v>64.84399999999999</v>
       </c>
       <c r="G13" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H13" t="n">
         <v>1.82</v>
       </c>
       <c r="I13" t="n">
-        <v>9.203390906781813</v>
+        <v>8.282946622471139</v>
       </c>
       <c r="J13" t="n">
-        <v>9.578947368421053</v>
+        <v>8.666666666666668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>